<commit_message>
Prints dos resultados de varios testes
</commit_message>
<xml_diff>
--- a/Analise/Roteiros.xlsx
+++ b/Analise/Roteiros.xlsx
@@ -3,17 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19415"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4465F973-CF77-447D-874A-99E371C71A08}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F0F4609-931A-4DE7-A0CE-B1CEFE0041F8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 Entregador" sheetId="3" r:id="rId1"/>
     <sheet name="2 Entregadores" sheetId="1" r:id="rId2"/>
     <sheet name="3 Entregadores" sheetId="2" r:id="rId3"/>
     <sheet name="4 Entregadores" sheetId="4" r:id="rId4"/>
-    <sheet name="Não é possível com apenas 1" sheetId="7" r:id="rId5"/>
-    <sheet name="Não é realizar a rota" sheetId="5" r:id="rId6"/>
+    <sheet name="Não é realizar a rota" sheetId="5" r:id="rId5"/>
+    <sheet name="Não é possível com apenas 1" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179016"/>
 </workbook>
@@ -157,6 +157,48 @@
     <t>Bertioga, SP, Brasil</t>
   </si>
   <si>
+    <t>Av. Paulista, 2355 - Bela Vista, São Paulo - SP</t>
+  </si>
+  <si>
+    <t>Praça da Sé - Sé, São Paulo - SP</t>
+  </si>
+  <si>
+    <t>Av. Jorn. Roberto Marinho, 85 - Cidade Monções, São Paulo - SP</t>
+  </si>
+  <si>
+    <t>Pq. Dom Pedro II - Av. Mercúrio, s/n - Brás, São Paulo - SP</t>
+  </si>
+  <si>
+    <t>R. Huet Bacelar, 407 - Ipiranga, São Paulo - SP</t>
+  </si>
+  <si>
+    <t>Parque da Independência - s/n - Ipiranga, São Paulo - SP</t>
+  </si>
+  <si>
+    <t>Av. Pedro Álvares Cabral - Vila Mariana, São Paulo - SP</t>
+  </si>
+  <si>
+    <t>Av. Miguel Estefno, 4241 - Vila Santo Estefano, São Paulo - SP</t>
+  </si>
+  <si>
+    <t>Av. Miguel Estefno, 3031 - Vila Água Funda, São Paulo - SP</t>
+  </si>
+  <si>
+    <t>Pç. Pateo do Collegio, 2 - Centro, São Paulo - SP</t>
+  </si>
+  <si>
+    <t>R. do Horto, 931 - Horto Florestal, São Paulo - SP</t>
+  </si>
+  <si>
+    <t>R. Antônio Cardoso Nogueira, 539 - Vila Chica Luisa, São Paulo - SP</t>
+  </si>
+  <si>
+    <t>Av. Sen. Teotônio Vilela, 261 - Interlagos, São Paulo - SP</t>
+  </si>
+  <si>
+    <t>Av. Olavo Fontoura, 1209 - Santana, São Paulo - SP</t>
+  </si>
+  <si>
     <t>Rua Maria Roschel Schunck, 817</t>
   </si>
   <si>
@@ -182,48 +224,6 @@
   </si>
   <si>
     <t>Catavento Cultural e Educacional - Avenida Mercúrio - Brás</t>
-  </si>
-  <si>
-    <t>Av. Paulista, 2355 - Bela Vista, São Paulo - SP</t>
-  </si>
-  <si>
-    <t>Praça da Sé - Sé, São Paulo - SP</t>
-  </si>
-  <si>
-    <t>Av. Jorn. Roberto Marinho, 85 - Cidade Monções, São Paulo - SP</t>
-  </si>
-  <si>
-    <t>Pq. Dom Pedro II - Av. Mercúrio, s/n - Brás, São Paulo - SP</t>
-  </si>
-  <si>
-    <t>R. Huet Bacelar, 407 - Ipiranga, São Paulo - SP</t>
-  </si>
-  <si>
-    <t>Parque da Independência - s/n - Ipiranga, São Paulo - SP</t>
-  </si>
-  <si>
-    <t>Av. Pedro Álvares Cabral - Vila Mariana, São Paulo - SP</t>
-  </si>
-  <si>
-    <t>Av. Miguel Estefno, 4241 - Vila Santo Estefano, São Paulo - SP</t>
-  </si>
-  <si>
-    <t>Av. Miguel Estefno, 3031 - Vila Água Funda, São Paulo - SP</t>
-  </si>
-  <si>
-    <t>Pç. Pateo do Collegio, 2 - Centro, São Paulo - SP</t>
-  </si>
-  <si>
-    <t>R. do Horto, 931 - Horto Florestal, São Paulo - SP</t>
-  </si>
-  <si>
-    <t>R. Antônio Cardoso Nogueira, 539 - Vila Chica Luisa, São Paulo - SP</t>
-  </si>
-  <si>
-    <t>Av. Sen. Teotônio Vilela, 261 - Interlagos, São Paulo - SP</t>
-  </si>
-  <si>
-    <t>Av. Olavo Fontoura, 1209 - Santana, São Paulo - SP</t>
   </si>
 </sst>
 </file>
@@ -600,7 +600,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" xr3:uid="{A1AAE3E1-3D71-542E-A14A-1CDC76F59A34}">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -640,7 +640,7 @@
         <v>0.375</v>
       </c>
       <c r="D2" s="1">
-        <v>0.75</v>
+        <v>0.79166666666666663</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -657,7 +657,7 @@
         <v>0.95833333333333337</v>
       </c>
       <c r="E3" s="4">
-        <v>120</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -978,7 +978,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0" xr3:uid="{8B8A21D1-FE79-5214-B4FC-70556F5A9641}">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1018,7 +1018,7 @@
         <v>0.25</v>
       </c>
       <c r="D2" s="1">
-        <v>0.91666666666666663</v>
+        <v>0.95833333333333337</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1217,8 +1217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B00D6F3-6017-4E97-875D-029F4BFCF546}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{635FFA52-AB88-5F44-A4E3-363D4B022FB4}">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0" xr3:uid="{635FFA52-AB88-5F44-A4E3-363D4B022FB4}">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1258,7 +1258,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D2" s="1">
-        <v>0.95833333333333337</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1420,11 +1420,285 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85F39743-6B1B-43CB-9860-13D38ACD78C2}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" xr3:uid="{D26CE0BF-2348-5A20-8C3E-B986FE8E7F44}">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.95833333333333337</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="E3" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="E4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E5" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E7" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="E8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E9" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0.6875</v>
+      </c>
+      <c r="E11" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="E12">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E13" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E14">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="4">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E15" s="4">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E112560-D7F3-4AAD-83DD-827E1A6B3B29}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{A96C06BA-33E8-5923-B356-9C228541379A}">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{A96C06BA-33E8-5923-B356-9C228541379A}">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1458,13 +1732,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="C2" s="1">
         <v>0.25</v>
       </c>
       <c r="D2" s="1">
-        <v>0.95833333333333337</v>
+        <v>0.80555555555555547</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1472,7 +1746,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="C3" s="5">
         <v>0.33333333333333331</v>
@@ -1489,7 +1763,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C4" s="1">
         <v>0.5</v>
@@ -1506,7 +1780,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="C5" s="5">
         <v>0.5</v>
@@ -1523,7 +1797,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="C6" s="1">
         <v>0.5</v>
@@ -1540,7 +1814,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="C7" s="5">
         <v>0.5</v>
@@ -1557,7 +1831,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="C8" s="1">
         <v>0.5</v>
@@ -1574,7 +1848,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="C9" s="5">
         <v>0.5</v>
@@ -1591,7 +1865,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="C10" s="1">
         <v>0.5</v>
@@ -1601,280 +1875,6 @@
       </c>
       <c r="E10">
         <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85F39743-6B1B-43CB-9860-13D38ACD78C2}">
-  <dimension ref="A1:E15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{D26CE0BF-2348-5A20-8C3E-B986FE8E7F44}">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0.375</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0.95833333333333337</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0.99930555555555556</v>
-      </c>
-      <c r="E3" s="4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.99930555555555556</v>
-      </c>
-      <c r="E4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="4">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0.375</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="E5" s="4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.375</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="E6">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="4">
-        <v>5</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0.375</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="E7" s="4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.99930555555555556</v>
-      </c>
-      <c r="E8">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="4">
-        <v>7</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="5">
-        <v>0.375</v>
-      </c>
-      <c r="D9" s="5">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="E9" s="4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.375</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="E10">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="4">
-        <v>9</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="5">
-        <v>0.375</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0.6875</v>
-      </c>
-      <c r="E11" s="4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="E12">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="4">
-        <v>11</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="5">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="E13" s="4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="E14">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="4">
-        <v>13</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="5">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="D15" s="5">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="E15" s="4">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Melhor organização das pastas de analise, geração dos dados dos teste 1,2 e 3. Criação de mapas para cada roteiro
</commit_message>
<xml_diff>
--- a/Analise/Roteiros.xlsx
+++ b/Analise/Roteiros.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19423"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F0F4609-931A-4DE7-A0CE-B1CEFE0041F8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DED052B4-F22B-4630-9557-91B7D78B7C15}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 Entregador" sheetId="3" r:id="rId1"/>
@@ -600,7 +600,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" xr3:uid="{A1AAE3E1-3D71-542E-A14A-1CDC76F59A34}">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -789,7 +789,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -977,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9B4359-0310-4824-9684-7E212A325D14}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{8B8A21D1-FE79-5214-B4FC-70556F5A9641}">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{8B8A21D1-FE79-5214-B4FC-70556F5A9641}">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1035,7 +1035,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="E3" s="4">
-        <v>320</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1052,7 +1052,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="E4">
-        <v>200</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1069,7 +1069,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="E5" s="4">
-        <v>360</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1086,7 +1086,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="E6">
-        <v>150</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1154,7 +1154,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="E10">
-        <v>500</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1188,7 +1188,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="E12">
-        <v>160</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1205,7 +1205,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="E13" s="4">
-        <v>120</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1218,7 +1218,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0" xr3:uid="{635FFA52-AB88-5F44-A4E3-363D4B022FB4}">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1424,7 +1424,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0" xr3:uid="{D26CE0BF-2348-5A20-8C3E-B986FE8E7F44}">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1697,7 +1697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E112560-D7F3-4AAD-83DD-827E1A6B3B29}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{A96C06BA-33E8-5923-B356-9C228541379A}">
+    <sheetView workbookViewId="0" xr3:uid="{A96C06BA-33E8-5923-B356-9C228541379A}">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adicao de descricao de imagens
</commit_message>
<xml_diff>
--- a/Analise/Roteiros.xlsx
+++ b/Analise/Roteiros.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19423"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DED052B4-F22B-4630-9557-91B7D78B7C15}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\d\SenacTCC\Analise\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA44BC55-81BB-4ADB-8B6F-5BC53A4B577A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 Entregador" sheetId="3" r:id="rId1"/>
@@ -14,13 +19,14 @@
     <sheet name="4 Entregadores" sheetId="4" r:id="rId4"/>
     <sheet name="Não é realizar a rota" sheetId="5" r:id="rId5"/>
     <sheet name="Não é possível com apenas 1" sheetId="7" r:id="rId6"/>
+    <sheet name="Planilha1" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179016"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="71">
   <si>
     <t>#</t>
   </si>
@@ -224,13 +230,22 @@
   </si>
   <si>
     <t>Catavento Cultural e Educacional - Avenida Mercúrio - Brás</t>
+  </si>
+  <si>
+    <t>Metrô Consolação - Avenida Paulista - Cerqueira César, São Paulo - SP, Brasil</t>
+  </si>
+  <si>
+    <t>Manaus, AM, Brasil</t>
+  </si>
+  <si>
+    <t>Minas Gerais, Brasil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,7 +316,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -599,20 +614,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143AC927-6C2A-48A5-871B-F586477FEA26}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{A1AAE3E1-3D71-542E-A14A-1CDC76F59A34}">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -629,7 +644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -643,7 +658,7 @@
         <v>0.79166666666666663</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -660,7 +675,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -677,7 +692,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -694,7 +709,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -711,7 +726,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -728,7 +743,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -745,7 +760,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -762,7 +777,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -788,20 +803,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -818,7 +833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -832,7 +847,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -849,7 +864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -866,7 +881,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -883,7 +898,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -900,7 +915,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -917,7 +932,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -934,7 +949,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -951,7 +966,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -977,20 +992,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9B4359-0310-4824-9684-7E212A325D14}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{8B8A21D1-FE79-5214-B4FC-70556F5A9641}">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1007,7 +1022,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1021,7 +1036,7 @@
         <v>0.95833333333333337</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1038,7 +1053,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1055,7 +1070,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -1072,7 +1087,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1089,7 +1104,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1106,7 +1121,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1123,7 +1138,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -1140,7 +1155,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1157,7 +1172,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -1174,7 +1189,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1191,7 +1206,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -1217,20 +1232,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B00D6F3-6017-4E97-875D-029F4BFCF546}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{635FFA52-AB88-5F44-A4E3-363D4B022FB4}">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1247,7 +1262,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1261,7 +1276,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1278,7 +1293,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1295,7 +1310,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -1312,7 +1327,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1329,7 +1344,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1346,7 +1361,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1363,7 +1378,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -1380,7 +1395,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1397,7 +1412,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -1423,20 +1438,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85F39743-6B1B-43CB-9860-13D38ACD78C2}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{D26CE0BF-2348-5A20-8C3E-B986FE8E7F44}">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1453,7 +1468,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1467,7 +1482,7 @@
         <v>0.95833333333333337</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1484,7 +1499,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1501,7 +1516,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -1518,7 +1533,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1535,7 +1550,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1552,7 +1567,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1569,7 +1584,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -1586,7 +1601,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1603,7 +1618,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -1620,7 +1635,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1637,7 +1652,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -1654,7 +1669,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1671,7 +1686,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -1697,20 +1712,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E112560-D7F3-4AAD-83DD-827E1A6B3B29}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{A96C06BA-33E8-5923-B356-9C228541379A}">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1727,7 +1742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1741,7 +1756,7 @@
         <v>0.80555555555555547</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1758,7 +1773,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1775,7 +1790,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -1792,7 +1807,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1809,7 +1824,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1826,7 +1841,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1843,7 +1858,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -1860,7 +1875,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1880,4 +1895,84 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA530BA9-6E03-4AE2-A196-F12DB9364C2C}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="67.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>